<commit_message>
working one link parser
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="21">
   <si>
     <t>postDay</t>
   </si>
@@ -68,8 +68,12 @@
     <t>[]</t>
   </si>
   <si>
-    <t xml:space="preserve">
-            Hello Loved ones,  </t>
+    <t>4242655324</t>
+  </si>
+  <si>
+    <t>Hello Loved ones,  I am a passionate, warm and experienced tantrika. I create a healing and intimate space for my guests. I am firm and deep with my technique, and I move gracefully and gently. I am certified in Lomi-Lomi and Reiki and also offer aromatherapy and crystal healing to leave you entirely balanced and at ease.    Hours: 12-8 PM
+Offering 60 &amp; 90 min.
+Call/Text: (424) 265-5324</t>
   </si>
   <si>
     <t>Blissful Goddess with Loving Hands</t>
@@ -433,42 +437,42 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:12">
-      <c s="1" r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c s="1" r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c s="1" r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c s="1" r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c s="1" r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c s="1" r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c s="1" r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c s="1" r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c s="1" r="J1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c s="1" r="K1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c s="1" r="L1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:12">
-      <c s="1" r="A2" t="n">
+      <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
       <c r="B2" t="s">
@@ -489,18 +493,20 @@
       <c r="G2" t="s">
         <v>16</v>
       </c>
-      <c r="H2" t="s"/>
+      <c r="H2" t="s">
+        <v>17</v>
+      </c>
       <c r="I2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J2" t="n">
         <v>1558</v>
       </c>
       <c r="K2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>